<commit_message>
First Succesfull TIM-AGRo deployment
</commit_message>
<xml_diff>
--- a/iCelerium/Content/UploadedFolder/TestAgent.xlsx
+++ b/iCelerium/Content/UploadedFolder/TestAgent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18080" yWindow="300" windowWidth="18400" windowHeight="7760"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Zone</t>
   </si>
@@ -39,62 +39,50 @@
     <t>Zone A</t>
   </si>
   <si>
-    <t>NAYO</t>
-  </si>
-  <si>
-    <t>Zone B</t>
-  </si>
-  <si>
-    <t>TAKELE</t>
-  </si>
-  <si>
     <t>ODETTE</t>
   </si>
   <si>
-    <t>Zone C</t>
-  </si>
-  <si>
     <t>AJAVON</t>
   </si>
   <si>
     <t>AKOESSO</t>
   </si>
   <si>
-    <t>Zone D</t>
-  </si>
-  <si>
     <t>YAWA</t>
   </si>
   <si>
     <t>KUDZU</t>
   </si>
   <si>
-    <t>Zone E</t>
-  </si>
-  <si>
-    <t>AFI</t>
-  </si>
-  <si>
-    <t>SYSLVIA</t>
-  </si>
-  <si>
-    <t>Zone F</t>
-  </si>
-  <si>
-    <t>GON</t>
-  </si>
-  <si>
-    <t>Zone G</t>
-  </si>
-  <si>
     <t>YVES</t>
+  </si>
+  <si>
+    <t>HERMANN</t>
+  </si>
+  <si>
+    <t>AHOOMEY</t>
+  </si>
+  <si>
+    <t>ELIE</t>
+  </si>
+  <si>
+    <t>SYLVIA</t>
+  </si>
+  <si>
+    <t>ALEX</t>
+  </si>
+  <si>
+    <t>DADA</t>
+  </si>
+  <si>
+    <t>GAVA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,22 +114,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,6 +148,19 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -182,9 +184,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -469,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -490,10 +492,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -513,10 +515,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>228</v>
@@ -524,10 +526,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>228</v>
@@ -535,10 +537,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>228</v>
@@ -546,10 +548,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>228</v>
@@ -557,10 +559,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>228</v>
@@ -568,10 +570,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>228</v>
@@ -579,10 +581,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>228</v>
@@ -590,10 +592,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>228</v>
@@ -601,10 +603,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>228</v>
@@ -612,10 +614,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>228</v>
@@ -623,18 +625,39 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C13">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
         <v>228</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>